<commit_message>
AutoCommit_17 июня 2024 г. 10:07:24_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>2ИСИП-522: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>изм</t>
+  </si>
+  <si>
+    <t xml:space="preserve">изм </t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -831,23 +834,26 @@
         <v>5</v>
       </c>
       <c r="G9" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H9" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I9" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J9" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M9">
         <v>3</v>
+      </c>
+      <c r="O9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 10:09:29_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -557,10 +557,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1422,20 +1422,20 @@
         <v>5</v>
       </c>
       <c r="G24" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I24" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J24" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L24">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M24">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 11:38:05_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -560,7 +560,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -996,17 +996,17 @@
         <v>5</v>
       </c>
       <c r="H13" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I13" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J13" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="M13">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_17 июня 2024 г. 18:04:55_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>2ИСИП-522: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t xml:space="preserve">изм </t>
+  </si>
+  <si>
+    <t>Осталось</t>
   </si>
 </sst>
 </file>
@@ -557,10 +560,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -606,14 +609,33 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="M3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="4" spans="1:15" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">

</xml_diff>

<commit_message>
AutoCommit_20 июня 2024 г. 14:15:13_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -551,10 +551,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N26" sqref="N26"/>
+      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1474,14 +1474,14 @@
         <v>5</v>
       </c>
       <c r="J25" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="M25">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O25" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
AutoCommit_20 июня 2024 г. 14:15:48_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -551,10 +551,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
+      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1462,7 +1462,7 @@
         <v>5</v>
       </c>
       <c r="F25" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G25" s="3">
         <v>5</v>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="L25">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="M25">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_21 июня 2024 г. 9:22:01_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -551,10 +551,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G25" sqref="G25"/>
+      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1562,7 +1562,10 @@
         <v>28</v>
       </c>
       <c r="M27">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="O27">
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_21 июня 2024 г. 22:31:27_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>2ИСИП-522: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>Сумма</t>
+  </si>
+  <si>
+    <t>ТК_оригинал</t>
+  </si>
+  <si>
+    <t>на момент выгрузки в элжуре</t>
   </si>
 </sst>
 </file>
@@ -216,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -241,6 +247,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -548,10 +557,10 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="G18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="P28" sqref="P28"/>
+      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -595,6 +604,12 @@
       <c r="L2" t="s">
         <v>36</v>
       </c>
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="O2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="3" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1">
@@ -660,7 +675,7 @@
       <c r="M4">
         <v>5</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="10">
         <v>4</v>
       </c>
       <c r="P4">
@@ -706,7 +721,7 @@
       <c r="M5">
         <v>5</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="10">
         <v>5</v>
       </c>
       <c r="P5">
@@ -714,7 +729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -753,7 +768,7 @@
       <c r="M6">
         <v>3</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="10">
         <v>4</v>
       </c>
       <c r="P6">
@@ -761,7 +776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -799,7 +814,7 @@
       <c r="M7">
         <v>5</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="10">
         <v>3</v>
       </c>
       <c r="P7">
@@ -807,7 +822,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -845,7 +860,7 @@
       <c r="M8">
         <v>5</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="10">
         <v>4</v>
       </c>
       <c r="P8">
@@ -853,7 +868,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -891,7 +906,7 @@
       <c r="M9">
         <v>5</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="10">
         <v>5</v>
       </c>
       <c r="P9">
@@ -899,7 +914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -937,7 +952,7 @@
       <c r="M10">
         <v>5</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="10">
         <v>5</v>
       </c>
       <c r="P10">
@@ -945,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -983,7 +998,7 @@
       <c r="M11">
         <v>5</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="10">
         <v>5</v>
       </c>
       <c r="P11">
@@ -991,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -1029,7 +1044,7 @@
       <c r="M12">
         <v>5</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="10">
         <v>5</v>
       </c>
       <c r="P12">
@@ -1037,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -1075,7 +1090,7 @@
       <c r="M13">
         <v>5</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="10">
         <v>5</v>
       </c>
       <c r="P13">
@@ -1083,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -1121,7 +1136,7 @@
       <c r="M14">
         <v>5</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="10">
         <v>5</v>
       </c>
       <c r="P14">
@@ -1129,7 +1144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -1167,7 +1182,7 @@
       <c r="M15">
         <v>5</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="10">
         <v>5</v>
       </c>
       <c r="P15">
@@ -1175,7 +1190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -1213,7 +1228,7 @@
       <c r="M16">
         <v>5</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="10">
         <v>5</v>
       </c>
       <c r="P16">
@@ -1221,7 +1236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -1259,7 +1274,7 @@
       <c r="M17">
         <v>3</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="10">
         <v>3</v>
       </c>
       <c r="P17">
@@ -1267,7 +1282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -1305,7 +1320,7 @@
       <c r="M18">
         <v>5</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="10">
         <v>4</v>
       </c>
       <c r="P18">
@@ -1313,7 +1328,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -1351,7 +1366,7 @@
       <c r="M19">
         <v>5</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="10">
         <v>5</v>
       </c>
       <c r="P19">
@@ -1359,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -1397,7 +1412,7 @@
       <c r="M20">
         <v>5</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="10">
         <v>5</v>
       </c>
       <c r="P20">
@@ -1405,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -1443,7 +1458,7 @@
       <c r="M21">
         <v>5</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="10">
         <v>3</v>
       </c>
       <c r="P21">
@@ -1451,7 +1466,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -1489,7 +1504,7 @@
       <c r="M22">
         <v>5</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="10">
         <v>5</v>
       </c>
       <c r="P22">
@@ -1497,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -1535,7 +1550,7 @@
       <c r="M23">
         <v>5</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="10">
         <v>5</v>
       </c>
       <c r="P23">
@@ -1543,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -1581,7 +1596,7 @@
       <c r="M24">
         <v>5</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="10">
         <v>5</v>
       </c>
       <c r="P24">
@@ -1589,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1627,7 +1642,7 @@
       <c r="M25">
         <v>5</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="10">
         <v>5</v>
       </c>
       <c r="P25">
@@ -1635,7 +1650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1673,7 +1688,7 @@
       <c r="M26">
         <v>4</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="10">
         <v>5</v>
       </c>
       <c r="P26">
@@ -1681,7 +1696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1719,7 +1734,7 @@
       <c r="M27">
         <v>4</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="10">
         <v>5</v>
       </c>
       <c r="P27">
@@ -1727,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1765,7 +1780,7 @@
       <c r="M28">
         <v>5</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="10">
         <v>3</v>
       </c>
       <c r="P28">
@@ -1773,7 +1788,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1811,7 +1826,7 @@
       <c r="M29">
         <v>4</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="10">
         <v>5</v>
       </c>
       <c r="P29">
@@ -1819,7 +1834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1857,7 +1872,7 @@
       <c r="M30">
         <v>5</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="10">
         <v>3</v>
       </c>
       <c r="P30">
@@ -1865,7 +1880,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1903,7 +1918,7 @@
       <c r="M31">
         <v>5</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="10">
         <v>4</v>
       </c>
       <c r="P31">
@@ -1911,7 +1926,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1949,7 +1964,7 @@
       <c r="M32">
         <v>5</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="10">
         <v>5</v>
       </c>
       <c r="P32">
@@ -1957,7 +1972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" ht="13" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>

</xml_diff>

<commit_message>
AutoCommit_23 июня 2024 г. 18:43:13_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522_ТерВер.xlsx
@@ -222,7 +222,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -248,6 +248,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -557,10 +560,10 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -627,15 +630,10 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-      <c r="I3" s="1">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="2"/>
+      <c r="M3" s="11"/>
     </row>
     <row r="4" spans="1:16" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">

</xml_diff>